<commit_message>
final-ish draft of preliminary model runs
</commit_message>
<xml_diff>
--- a/Model Data Sheets and Code/preliminary_model_results.xlsx
+++ b/Model Data Sheets and Code/preliminary_model_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amlpa\OneDrive\2019 Work shit\zaca-mcf-manuscript\Model Data Sheets and Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02242997-3945-451E-A967-DE293C5E5C2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684509A4-529F-41B8-B5A6-5B55C1D5BDC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2F1CA497-3FDB-467D-8ED1-3B4A3868D9BD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="83">
   <si>
     <t>Model</t>
   </si>
@@ -175,9 +175,6 @@
     <t>removed the moderate class. Carla and another professor agreed its okay if we are looking at the extremes (high v none/low); While the OOB is only 25% for high mortality stands, the PDP shows that the ability of the model to correctly predict high = ~ 0%  or is very negative (just looked at the most important variables), so I interpret this as the model cannot distinguish/predict high mortality stands, instead it is just basing its predicitve power entirely on the none/low class and whenever its ability to predict none/low decreases it just assumes it is the other mortality class; ALE plots do not have this issue</t>
   </si>
   <si>
-    <t>slope, precip, january vpd</t>
-  </si>
-  <si>
     <t>pretty stable!</t>
   </si>
   <si>
@@ -187,9 +184,6 @@
     <t>see cell 6G</t>
   </si>
   <si>
-    <t>Manual mortality (type converted)</t>
-  </si>
-  <si>
     <t>non type converted = 17, type converted = 26%</t>
   </si>
   <si>
@@ -284,13 +278,85 @@
   </si>
   <si>
     <t>auc=91.8%</t>
+  </si>
+  <si>
+    <t>Manual mortality: type conversion</t>
+  </si>
+  <si>
+    <t>not that stable :/</t>
+  </si>
+  <si>
+    <t>slope, precip, august vpd</t>
+  </si>
+  <si>
+    <t>slope, vpd_aug, elevation</t>
+  </si>
+  <si>
+    <t>auc=88.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pretty stable. </t>
+  </si>
+  <si>
+    <t>variable importance is a Lot more stable than the forced sample size trial, but the type converted class accuracy is awful</t>
+  </si>
+  <si>
+    <t>vpd_aug, slope, precip</t>
+  </si>
+  <si>
+    <t>Manual mortality: type conversion (mcf)</t>
+  </si>
+  <si>
+    <t>rdnbr: type conversion (pico)</t>
+  </si>
+  <si>
+    <t>rdnbr: type conversion (mcf + pico)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">non type converted = 0%, type converted = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>91%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">non type converted = 3%, type converted = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>72%</t>
+    </r>
+  </si>
+  <si>
+    <t>rdnbr: type conversion (mcf)-using threshold</t>
+  </si>
+  <si>
+    <t>pretty sure I did not go about the right way of picking a threshold.</t>
+  </si>
+  <si>
+    <t>cant do</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,6 +376,13 @@
       <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -341,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -360,6 +433,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -675,11 +751,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B60CFD82-0EBB-47CF-A85B-690511E2D58D}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -835,172 +911,235 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1">
+        <v>150</v>
+      </c>
+      <c r="C7" s="1">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="1">
-        <v>99</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0.18</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="1">
-        <v>150</v>
-      </c>
-      <c r="C8" s="1">
-        <v>20</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>40</v>
+      <c r="D8" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>46</v>
+        <v>53</v>
+      </c>
+      <c r="B10" s="1">
+        <v>326</v>
+      </c>
+      <c r="C10" s="1">
+        <v>18.5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="1">
-        <v>326</v>
-      </c>
-      <c r="C11" s="1">
-        <v>18.5</v>
-      </c>
-      <c r="D11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="1">
+        <v>863</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.16</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="1">
+        <v>99</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.12</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" s="1">
-        <v>863</v>
-      </c>
-      <c r="C13" s="5">
-        <v>0.16</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    </row>
+    <row r="16" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>